<commit_message>
Adding a data in excelsheet and java program
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="22980" windowHeight="9024" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17880" windowHeight="3855"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="3" r:id="rId1"/>
     <sheet name="php" sheetId="2" r:id="rId2"/>
     <sheet name="Test" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>1</t>
   </si>
@@ -70,13 +71,82 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Email id</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>Birthmonth</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Cityname</t>
+  </si>
+  <si>
+    <t>Statename</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>venkatesh</t>
+  </si>
+  <si>
+    <t>baskar</t>
+  </si>
+  <si>
+    <t>it trident</t>
+  </si>
+  <si>
+    <t>5.IT trident ,northusman road ,3rd floor,tnagar,chennai</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>venkateshbaskar22+14@gmail.com</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>61291</t>
+  </si>
+  <si>
+    <t>9585153985</t>
+  </si>
+  <si>
+    <t>1234567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +157,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF484C55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,10 +194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,8 +209,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,15 +522,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -440,11 +641,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -454,17 +655,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added validation for swaglab test
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>1</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Sort</t>
+  </si>
+  <si>
+    <t>lohi</t>
+  </si>
+  <si>
+    <t>hilo</t>
   </si>
 </sst>
 </file>
@@ -452,10 +461,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +476,7 @@
     <col min="6" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -489,8 +498,11 @@
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -512,8 +524,11 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -534,6 +549,9 @@
       </c>
       <c r="G3" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked on the project as said.
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -219,10 +219,10 @@
     <t>30</t>
   </si>
   <si>
-    <t xml:space="preserve"> McCarran</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chennai</t>
+    <t>McCarran</t>
+  </si>
+  <si>
+    <t>Chennai</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated gitignore and added allure dependencies.
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="20730" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13830" windowHeight="6150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="3" r:id="rId1"/>
     <sheet name="php" sheetId="2" r:id="rId2"/>
     <sheet name="Test" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I19"/>
 </workbook>
 </file>
 
@@ -594,7 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -822,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
To take a pull from develop
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="1" r:id="rId1"/>
     <sheet name="php" sheetId="2" r:id="rId2"/>
     <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="C1:N22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>Number</t>
   </si>
@@ -292,12 +293,6 @@
   </si>
   <si>
     <t>hilo</t>
-  </si>
-  <si>
-    <t>nill</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Pass</t>
@@ -307,7 +302,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -665,19 +659,19 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.88671875"/>
-    <col min="2" max="2" customWidth="true" width="15.6640625"/>
-    <col min="3" max="3" customWidth="true" width="14.21875"/>
-    <col min="4" max="4" customWidth="true" width="18.21875"/>
-    <col min="5" max="5" customWidth="true" width="12.0"/>
-    <col min="6" max="6" customWidth="true" width="18.77734375"/>
-    <col min="7" max="8" customWidth="true" width="14.44140625"/>
-    <col min="9" max="9" customWidth="true" width="18.88671875"/>
-    <col min="10" max="10" customWidth="true" width="17.77734375"/>
-    <col min="11" max="12" customWidth="true" width="14.33203125"/>
-    <col min="13" max="13" customWidth="true" width="15.109375"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -775,27 +769,27 @@
       <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.21875"/>
-    <col min="2" max="2" customWidth="true" width="12.109375"/>
-    <col min="3" max="3" customWidth="true" width="13.77734375"/>
-    <col min="4" max="4" customWidth="true" width="11.88671875"/>
-    <col min="5" max="5" customWidth="true" width="16.109375"/>
-    <col min="6" max="6" customWidth="true" width="11.88671875"/>
-    <col min="7" max="7" customWidth="true" width="11.44140625"/>
-    <col min="10" max="10" customWidth="true" width="13.6640625"/>
-    <col min="11" max="11" customWidth="true" width="15.0"/>
-    <col min="12" max="12" customWidth="true" width="11.109375"/>
-    <col min="20" max="20" customWidth="true" width="12.77734375"/>
-    <col min="22" max="22" customWidth="true" width="12.21875"/>
-    <col min="23" max="23" customWidth="true" width="11.5546875"/>
-    <col min="24" max="24" customWidth="true" width="12.0"/>
-    <col min="25" max="25" customWidth="true" width="11.77734375"/>
-    <col min="26" max="26" customWidth="true" width="16.21875"/>
-    <col min="27" max="27" customWidth="true" width="11.5546875"/>
-    <col min="28" max="28" customWidth="true" width="14.21875"/>
-    <col min="29" max="29" customWidth="true" width="20.6640625"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="25" max="25" width="11.7109375" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" customWidth="1"/>
+    <col min="29" max="29" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -992,17 +986,17 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.33203125"/>
-    <col min="2" max="2" customWidth="true" width="21.33203125"/>
-    <col min="3" max="3" customWidth="true" width="15.33203125"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
-    <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="6" max="6" customWidth="true" width="11.109375"/>
-    <col min="7" max="7" customWidth="true" width="9.6640625"/>
-    <col min="8" max="8" customWidth="true" width="11.88671875"/>
-    <col min="9" max="9" customWidth="true" width="11.0"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1060,7 +1054,7 @@
         <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1089,7 +1083,7 @@
         <v>91</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Parallel execution issue
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="C1:N22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="92">
   <si>
     <t>Number</t>
   </si>
@@ -193,9 +192,6 @@
     <t>round trip</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -238,18 +234,12 @@
     <t>15,16,14,12,17</t>
   </si>
   <si>
-    <t>2031,2032,2033,2030,0000</t>
-  </si>
-  <si>
     <t>Gopi,Gowri,Gowshik,Gopika,Govinth</t>
   </si>
   <si>
     <t>Muthu,gopi,gopi,gopi,gopi</t>
   </si>
   <si>
-    <t>1.23456789009876E+49</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -296,6 +286,12 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>2031,2032,2033,2030,2031</t>
+  </si>
+  <si>
+    <t>1234567890,0987654321,6789054321,5432167890,1234560987</t>
   </si>
 </sst>
 </file>
@@ -765,31 +761,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="25" max="25" width="11.7109375" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" customWidth="1"/>
-    <col min="28" max="28" width="14.28515625" customWidth="1"/>
-    <col min="29" max="29" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
@@ -892,82 +895,82 @@
         <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
         <v>60</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" t="s">
         <v>63</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>64</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
         <v>65</v>
       </c>
-      <c r="P2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA2" t="s">
         <v>72</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AB2" t="s">
         <v>73</v>
       </c>
-      <c r="AA2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>75</v>
-      </c>
       <c r="AC2" s="5" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -982,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1004,28 +1007,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1033,57 +1036,57 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
         <v>89</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the parallel execution issue
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -180,118 +180,118 @@
     <t>passportid</t>
   </si>
   <si>
+    <t>round trip</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>test@mail.com</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>test street,test city</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>MR,MRS,MR,MISS,MR</t>
+  </si>
+  <si>
+    <t>01,02,03,04,05</t>
+  </si>
+  <si>
+    <t>11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>1999,2001,2015,2010,0000</t>
+  </si>
+  <si>
+    <t>11,22,13,14,15</t>
+  </si>
+  <si>
+    <t>2001,2002,2010,2010,0000</t>
+  </si>
+  <si>
+    <t>15,16,14,12,17</t>
+  </si>
+  <si>
+    <t>Gopi,Gowri,Gowshik,Gopika,Govinth</t>
+  </si>
+  <si>
+    <t>Muthu,gopi,gopi,gopi,gopi</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Sort</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Sowmya</t>
+  </si>
+  <si>
+    <t>Venkateshwaran</t>
+  </si>
+  <si>
+    <t>621714</t>
+  </si>
+  <si>
+    <t>lohi</t>
+  </si>
+  <si>
+    <t>621700</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>hilo</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>2031,2032,2033,2030,2031</t>
+  </si>
+  <si>
+    <t>1234567890,0987654321,6789054321,5432167890,1234560987</t>
+  </si>
+  <si>
     <t>Chennai</t>
   </si>
   <si>
     <t>McCarran</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>round trip</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Arun</t>
-  </si>
-  <si>
-    <t>Sachin</t>
-  </si>
-  <si>
-    <t>test@mail.com</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>test street,test city</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>MR,MRS,MR,MISS,MR</t>
-  </si>
-  <si>
-    <t>01,02,03,04,05</t>
-  </si>
-  <si>
-    <t>11,12,13,14,15</t>
-  </si>
-  <si>
-    <t>1999,2001,2015,2010,0000</t>
-  </si>
-  <si>
-    <t>11,22,13,14,15</t>
-  </si>
-  <si>
-    <t>2001,2002,2010,2010,0000</t>
-  </si>
-  <si>
-    <t>15,16,14,12,17</t>
-  </si>
-  <si>
-    <t>Gopi,Gowri,Gowshik,Gopika,Govinth</t>
-  </si>
-  <si>
-    <t>Muthu,gopi,gopi,gopi,gopi</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Sort</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>Sowmya</t>
-  </si>
-  <si>
-    <t>Venkateshwaran</t>
-  </si>
-  <si>
-    <t>621714</t>
-  </si>
-  <si>
-    <t>lohi</t>
-  </si>
-  <si>
-    <t>621700</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>hilo</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>2031,2032,2033,2030,2031</t>
-  </si>
-  <si>
-    <t>1234567890,0987654321,6789054321,5432167890,1234560987</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -762,7 +762,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,88 +889,88 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="O2" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P2" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="T2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="U2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="W2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="X2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="3" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" t="s">
         <v>69</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="AB2" t="s">
         <v>70</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>73</v>
-      </c>
       <c r="AC2" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1007,28 +1007,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1036,57 +1036,57 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" t="s">
         <v>86</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added changes in Swag_lab runner class
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
   <si>
     <t>Number</t>
   </si>
@@ -288,12 +288,6 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Test_1</t>
-  </si>
-  <si>
-    <t>Test_2</t>
-  </si>
-  <si>
     <t>Search flight</t>
   </si>
   <si>
@@ -304,12 +298,19 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Order Confirmation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -669,17 +670,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875"/>
+    <col min="2" max="2" customWidth="true" width="15.7109375"/>
+    <col min="3" max="3" customWidth="true" width="14.28515625"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625"/>
+    <col min="5" max="5" customWidth="true" width="12.0"/>
+    <col min="6" max="6" customWidth="true" width="18.7109375"/>
+    <col min="7" max="8" customWidth="true" width="14.42578125"/>
+    <col min="9" max="9" customWidth="true" width="18.85546875"/>
+    <col min="10" max="10" customWidth="true" width="17.7109375"/>
+    <col min="11" max="12" customWidth="true" width="14.28515625"/>
+    <col min="13" max="13" customWidth="true" width="15.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -773,39 +774,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.5703125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.28515625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.28515625"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.5703125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625"/>
+    <col min="18" max="19" bestFit="true" customWidth="true" width="13.42578125"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="23.7109375"/>
+    <col min="21" max="22" bestFit="true" customWidth="true" width="13.42578125"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.7109375"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" width="13.42578125"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="23.7109375"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="34.28515625"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="54.85546875"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
@@ -917,7 +918,7 @@
         <v>53</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>54</v>
@@ -989,7 +990,7 @@
         <v>86</v>
       </c>
       <c r="AD2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -1009,7 +1010,7 @@
         <v>53</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>54</v>
@@ -1081,7 +1082,7 @@
         <v>86</v>
       </c>
       <c r="AD3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1097,21 +1098,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="5" max="5" customWidth="true" width="16.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.42578125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1172,10 +1174,10 @@
         <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1204,10 +1206,10 @@
         <v>84</v>
       </c>
       <c r="I3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create a steps definition and pageobjects for cucumber
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14775" windowHeight="7215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15810" windowHeight="4335"/>
   </bookViews>
   <sheets>
     <sheet name="yolo" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:I13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
   <si>
     <t>Number</t>
   </si>
@@ -310,7 +311,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -664,23 +664,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.85546875"/>
-    <col min="2" max="2" customWidth="true" width="15.7109375"/>
-    <col min="3" max="3" customWidth="true" width="14.28515625"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625"/>
-    <col min="5" max="5" customWidth="true" width="12.0"/>
-    <col min="6" max="6" customWidth="true" width="18.7109375"/>
-    <col min="7" max="8" customWidth="true" width="14.42578125"/>
-    <col min="9" max="9" customWidth="true" width="18.85546875"/>
-    <col min="10" max="10" customWidth="true" width="17.7109375"/>
-    <col min="11" max="12" customWidth="true" width="14.28515625"/>
-    <col min="13" max="13" customWidth="true" width="15.140625"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -780,33 +780,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.0"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.5703125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.28515625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.28515625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.5703125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.140625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="14.5703125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.7109375"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="20.28515625"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" width="13.42578125"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="23.7109375"/>
-    <col min="21" max="22" bestFit="true" customWidth="true" width="13.42578125"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="23.7109375"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" width="13.42578125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="23.7109375"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="34.28515625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="25.0"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="54.85546875"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="12.0"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
@@ -1098,22 +1098,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.28515625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.7109375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
-    <col min="5" max="5" customWidth="true" width="16.0"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="4.5703125"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.42578125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.5703125"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Made changes to mail.class
</commit_message>
<xml_diff>
--- a/src/main/java/resources/excelsheet/database.xlsx
+++ b/src/main/java/resources/excelsheet/database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="97">
   <si>
     <t>Number</t>
   </si>
@@ -1177,7 +1177,7 @@
         <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>94</v>
@@ -1209,7 +1209,7 @@
         <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>95</v>

</xml_diff>